<commit_message>
new multiple_paternity excel spreadsheet, with new sheet for alfaro-nunez calculations
</commit_message>
<xml_diff>
--- a/data/multiple_paternity.xlsx
+++ b/data/multiple_paternity.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vique\Documents\Projects\iliketurtles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C170C445-4C50-45D4-98DD-D8023D38A8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FD2909-3617-414D-917C-EE5577BACF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6360" yWindow="3408" windowWidth="13824" windowHeight="7176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="alfaro-nunez" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
   <si>
     <t>Paper</t>
   </si>
@@ -79,13 +80,88 @@
   </si>
   <si>
     <t>sum_check</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Average hatchlings sampled</t>
+  </si>
+  <si>
+    <t>Percent hatchlings sampled</t>
+  </si>
+  <si>
+    <t>Nest</t>
+  </si>
+  <si>
+    <t>Sire 1</t>
+  </si>
+  <si>
+    <t>Sire 2</t>
+  </si>
+  <si>
+    <t>Sire 3</t>
+  </si>
+  <si>
+    <t>Sire 4</t>
+  </si>
+  <si>
+    <t>Sire 5</t>
+  </si>
+  <si>
+    <t>2 sires</t>
+  </si>
+  <si>
+    <t>3 sires</t>
+  </si>
+  <si>
+    <t>4 sires</t>
+  </si>
+  <si>
+    <t>5 sires</t>
+  </si>
+  <si>
+    <t>sire 1:</t>
+  </si>
+  <si>
+    <t>sire 2:</t>
+  </si>
+  <si>
+    <t>sire 3:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sire 1: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sire 2: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sire 3: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sire 4: </t>
+  </si>
+  <si>
+    <t>sire 5:</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>sum check</t>
+  </si>
+  <si>
+    <t>Original values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +177,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,9 +192,85 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -122,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -130,6 +288,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,15 +607,17 @@
     <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.21875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,25 +625,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -463,26 +657,32 @@
         <v>8</v>
       </c>
       <c r="C2" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
         <v>0.31034483000000002</v>
       </c>
-      <c r="D2" s="2">
+      <c r="F2" s="2">
         <v>0.44827586000000003</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="2">
         <v>0.17241379000000001</v>
       </c>
-      <c r="F2" s="2">
+      <c r="H2" s="2">
         <v>3.4482760000000001E-2</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="2">
         <v>3.4482760000000001E-2</v>
       </c>
-      <c r="H2" s="2">
-        <f>SUM(C2:G2)</f>
+      <c r="J2" s="3">
+        <f>SUM(E2:I2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -490,56 +690,68 @@
         <v>10</v>
       </c>
       <c r="C3" s="2">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2">
         <v>0.72340426000000002</v>
       </c>
-      <c r="D3" s="2">
+      <c r="F3" s="2">
         <v>0.21276596</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="2">
         <v>5.3191490000000001E-2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
         <v>1.06383E-2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H5" si="0">SUM(C3:G3)</f>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J5" si="0">SUM(E3:I3)</f>
         <v>1.0000000100000002</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
         <f>9/13</f>
         <v>0.69230769230769229</v>
       </c>
-      <c r="D4" s="2">
+      <c r="F4" s="2">
         <f>2/13</f>
         <v>0.15384615384615385</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="2">
         <f>2/13</f>
         <v>0.15384615384615385</v>
       </c>
-      <c r="F4" s="2">
+      <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -547,28 +759,693 @@
         <v>10</v>
       </c>
       <c r="C5" s="2">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" s="2">
         <f>4/12</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G5" s="2">
         <f>4/12</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F5" s="2">
+      <c r="H5" s="2">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <f>2/12</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="H5" s="2">
+      <c r="J5" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C6753A-7503-447F-A3F7-5695C28C3D94}">
+  <dimension ref="A1:T23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>54.85</v>
+      </c>
+      <c r="C4" s="7">
+        <v>29.92</v>
+      </c>
+      <c r="D4" s="7">
+        <v>15.23</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="10">
+        <v>4</v>
+      </c>
+      <c r="I4" s="10">
+        <v>95.01</v>
+      </c>
+      <c r="J4" s="10">
+        <v>4.99</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="12">
+        <f>AVERAGE(I4:I7)</f>
+        <v>88.677500000000009</v>
+      </c>
+      <c r="P4" s="12">
+        <f>AVERAGE(J4:J7)</f>
+        <v>11.3225</v>
+      </c>
+      <c r="T4">
+        <f>SUM(O4:P4)</f>
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>54.85</v>
+      </c>
+      <c r="C5" s="7">
+        <v>29.92</v>
+      </c>
+      <c r="D5" s="7">
+        <v>15.23</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="10">
+        <v>5</v>
+      </c>
+      <c r="I5" s="10">
+        <v>84.77</v>
+      </c>
+      <c r="J5" s="10">
+        <v>15.23</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>95.01</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4.99</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="10">
+        <v>8</v>
+      </c>
+      <c r="I6" s="10">
+        <v>95.01</v>
+      </c>
+      <c r="J6" s="10">
+        <v>4.99</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>84.77</v>
+      </c>
+      <c r="C7" s="7">
+        <v>15.23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="10">
+        <v>13</v>
+      </c>
+      <c r="I7" s="10">
+        <v>79.92</v>
+      </c>
+      <c r="J7" s="10">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>40.03</v>
+      </c>
+      <c r="C8" s="7">
+        <v>29.92</v>
+      </c>
+      <c r="D8" s="7">
+        <v>30.05</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>100</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>95.01</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4.99</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <v>54.85</v>
+      </c>
+      <c r="C11" s="7">
+        <v>25.08</v>
+      </c>
+      <c r="D11" s="7">
+        <v>15.09</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4.99</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10">
+        <v>54.85</v>
+      </c>
+      <c r="J11" s="10">
+        <v>29.92</v>
+      </c>
+      <c r="K11" s="10">
+        <v>15.23</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="T11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7">
+        <v>50</v>
+      </c>
+      <c r="C12" s="7">
+        <v>19.95</v>
+      </c>
+      <c r="D12" s="7">
+        <v>14.82</v>
+      </c>
+      <c r="E12" s="7">
+        <v>10.24</v>
+      </c>
+      <c r="F12" s="7">
+        <v>4.99</v>
+      </c>
+      <c r="H12" s="10">
+        <v>2</v>
+      </c>
+      <c r="I12" s="10">
+        <v>54.85</v>
+      </c>
+      <c r="J12" s="10">
+        <v>29.92</v>
+      </c>
+      <c r="K12" s="10">
+        <v>15.23</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="12">
+        <f>AVERAGE(I11:I14)</f>
+        <v>47.440000000000005</v>
+      </c>
+      <c r="P12" s="12">
+        <f>AVERAGE(J11:J14)</f>
+        <v>32.412500000000001</v>
+      </c>
+      <c r="Q12" s="12">
+        <f>AVERAGE(K11:K14)</f>
+        <v>20.147500000000001</v>
+      </c>
+      <c r="T12">
+        <f>SUM(O12:Q12)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7">
+        <v>40.03</v>
+      </c>
+      <c r="C13" s="7">
+        <v>39.89</v>
+      </c>
+      <c r="D13" s="7">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="10">
+        <v>6</v>
+      </c>
+      <c r="I13" s="10">
+        <v>40.03</v>
+      </c>
+      <c r="J13" s="10">
+        <v>29.92</v>
+      </c>
+      <c r="K13" s="10">
+        <v>30.05</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7">
+        <v>79.92</v>
+      </c>
+      <c r="C14" s="7">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="10">
+        <v>12</v>
+      </c>
+      <c r="I14" s="10">
+        <v>40.03</v>
+      </c>
+      <c r="J14" s="10">
+        <v>39.89</v>
+      </c>
+      <c r="K14" s="10">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <v>44.88</v>
+      </c>
+      <c r="C15" s="7">
+        <v>19.68</v>
+      </c>
+      <c r="D15" s="7">
+        <v>15.63</v>
+      </c>
+      <c r="E15" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F15" s="7">
+        <v>10.11</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="8:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H18" s="10">
+        <v>10</v>
+      </c>
+      <c r="I18" s="10">
+        <v>54.85</v>
+      </c>
+      <c r="J18" s="10">
+        <v>25.08</v>
+      </c>
+      <c r="K18" s="10">
+        <v>15.09</v>
+      </c>
+      <c r="L18" s="10">
+        <v>4.99</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O18" t="s">
+        <v>31</v>
+      </c>
+      <c r="P18" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>33</v>
+      </c>
+      <c r="R18" t="s">
+        <v>34</v>
+      </c>
+      <c r="T18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="8:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O19" s="9">
+        <v>54.85</v>
+      </c>
+      <c r="P19" s="9">
+        <v>25.08</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>15.09</v>
+      </c>
+      <c r="R19" s="9">
+        <v>4.99</v>
+      </c>
+      <c r="T19">
+        <f>SUM(I18:L18)</f>
+        <v>100.01</v>
+      </c>
+    </row>
+    <row r="20" spans="8:20" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="8:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H22" s="10">
+        <v>11</v>
+      </c>
+      <c r="I22" s="10">
+        <v>50</v>
+      </c>
+      <c r="J22" s="10">
+        <v>19.95</v>
+      </c>
+      <c r="K22" s="10">
+        <v>14.82</v>
+      </c>
+      <c r="L22" s="10">
+        <v>10.24</v>
+      </c>
+      <c r="M22" s="10">
+        <v>4.99</v>
+      </c>
+      <c r="O22" t="s">
+        <v>31</v>
+      </c>
+      <c r="P22" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>33</v>
+      </c>
+      <c r="R22" t="s">
+        <v>34</v>
+      </c>
+      <c r="S22" t="s">
+        <v>35</v>
+      </c>
+      <c r="T22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="8:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H23" s="10">
+        <v>14</v>
+      </c>
+      <c r="I23" s="10">
+        <v>44.88</v>
+      </c>
+      <c r="J23" s="10">
+        <v>19.68</v>
+      </c>
+      <c r="K23" s="10">
+        <v>15.63</v>
+      </c>
+      <c r="L23" s="10">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="M23" s="10">
+        <v>10.11</v>
+      </c>
+      <c r="O23" s="12">
+        <f>AVERAGE(I22:I23)</f>
+        <v>47.44</v>
+      </c>
+      <c r="P23" s="12">
+        <f>AVERAGE(J22:J23)</f>
+        <v>19.814999999999998</v>
+      </c>
+      <c r="Q23" s="12">
+        <f>AVERAGE(K22:K23)</f>
+        <v>15.225000000000001</v>
+      </c>
+      <c r="R23" s="12">
+        <f>AVERAGE(L22:L23)</f>
+        <v>9.9699999999999989</v>
+      </c>
+      <c r="S23" s="12">
+        <f>AVERAGE(M22:M23)</f>
+        <v>7.55</v>
+      </c>
+      <c r="T23">
+        <f>SUM(O23:S23)</f>
+        <v>99.999999999999986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>